<commit_message>
Started integrating other repo
Started the process of integrating the other repo that had a lot of the ONP and handrit related code. DB builder is also working agin now, but something else broke again
</commit_message>
<xml_diff>
--- a/data/ingest/monasteries.xlsx
+++ b/data/ingest/monasteries.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEF2693-6155-1648-A0C0-B9E103C56DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65E92E7-920A-BE41-89E2-4ECADA5F33A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="83">
   <si>
     <t>Name</t>
   </si>
@@ -260,6 +260,15 @@
   </si>
   <si>
     <t>nedlagt på 1200-tallet</t>
+  </si>
+  <si>
+    <t>Vadstena</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Vadstena kloster</t>
   </si>
 </sst>
 </file>
@@ -315,8 +324,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DF98C47-C10B-BE41-A45E-DF52A9C2F2B8}" name="Tabelle1" displayName="Tabelle1" ref="A1:J36" totalsRowShown="0">
-  <autoFilter ref="A1:J36" xr:uid="{3DF98C47-C10B-BE41-A45E-DF52A9C2F2B8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DF98C47-C10B-BE41-A45E-DF52A9C2F2B8}" name="Tabelle1" displayName="Tabelle1" ref="A1:J37" totalsRowShown="0">
+  <autoFilter ref="A1:J37" xr:uid="{3DF98C47-C10B-BE41-A45E-DF52A9C2F2B8}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J36">
     <sortCondition ref="B1:B36"/>
   </sortState>
@@ -599,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:G24"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1204,6 +1213,17 @@
         <v>18</v>
       </c>
     </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" t="s">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>